<commit_message>
Added Member Type and Salutation in Member Form
</commit_message>
<xml_diff>
--- a/Docs/Delivery_Details.xlsx
+++ b/Docs/Delivery_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NTCYNK\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A5BE6F-5C2D-464F-B635-FCF9B172D15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22952799-7CBA-4BF5-B7BF-60454CAB95FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,7 +137,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -235,11 +235,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -524,7 +524,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,35 +770,37 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>45026</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="2">
         <v>5</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5">
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>45168</v>
+      </c>
+      <c r="J7" s="2">
         <v>600</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="13">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
@@ -828,7 +830,9 @@
       <c r="H8" s="4">
         <v>1</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="3">
+        <v>45168</v>
+      </c>
       <c r="J8" s="2">
         <v>600</v>
       </c>
@@ -872,35 +876,37 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>45026</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="2">
         <v>4</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5">
+      <c r="G10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>45168</v>
+      </c>
+      <c r="J10" s="2">
         <v>600</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="13">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
@@ -940,37 +946,39 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="3">
         <v>45026</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="5">
-        <v>6</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5">
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>45168</v>
+      </c>
+      <c r="J12" s="2">
         <v>600</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="13">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1022,7 +1030,7 @@
       </c>
       <c r="K14" s="14">
         <f>SUM(K2:K13)</f>
-        <v>22200</v>
+        <v>21000</v>
       </c>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>

</xml_diff>

<commit_message>
Implemented Member Photo and Liquor Order Waiter
</commit_message>
<xml_diff>
--- a/Docs/Delivery_Details.xlsx
+++ b/Docs/Delivery_Details.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NTCYNK\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MurugesanG\Projects\NTCYNK\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22952799-7CBA-4BF5-B7BF-60454CAB95FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0820161-0399-4873-AC07-B99340979E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="45">
   <si>
     <t>Sr.No</t>
   </si>
@@ -128,7 +127,49 @@
     <t>Calculated Amount</t>
   </si>
   <si>
-    <t>Total Amount</t>
+    <t>Update Membership Type and Salutation in Database</t>
+  </si>
+  <si>
+    <t>Adding Member Photo in Member Form</t>
+  </si>
+  <si>
+    <t>Adding Member Documents in Member Form</t>
+  </si>
+  <si>
+    <t>Member Report with History</t>
+  </si>
+  <si>
+    <t>Adding Member History in Member Form (Date, Comments, Upload Image / PDF / Videos)</t>
+  </si>
+  <si>
+    <t>Yet to Start</t>
+  </si>
+  <si>
+    <t>Dropdown Waiter Name in Liquor Order Page</t>
+  </si>
+  <si>
+    <t>Sync the data between Primary and Secondary server</t>
+  </si>
+  <si>
+    <t>Total Hours and Charges</t>
+  </si>
+  <si>
+    <t>Room Booking Page</t>
+  </si>
+  <si>
+    <t>Room Booking Report</t>
+  </si>
+  <si>
+    <t>Estimated Amount</t>
+  </si>
+  <si>
+    <t>Billed Amount</t>
+  </si>
+  <si>
+    <t>Requested Date</t>
+  </si>
+  <si>
+    <t>Load the pre-defined Waiter Names in Liquor Order Page and Implement Validation</t>
   </si>
 </sst>
 </file>
@@ -136,8 +177,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -221,9 +262,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -235,11 +276,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -521,17 +568,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -627,6 +674,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
+        <f t="shared" ref="A3:A20" si="0">+A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="9">
@@ -657,12 +705,13 @@
         <v>0</v>
       </c>
       <c r="K3" s="11">
-        <f t="shared" ref="K3:K13" si="0">F3*J3</f>
+        <f t="shared" ref="K3:K11" si="1">F3*J3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="9">
@@ -693,12 +742,13 @@
         <v>0</v>
       </c>
       <c r="K4" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="9">
@@ -729,12 +779,13 @@
         <v>0</v>
       </c>
       <c r="K5" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="9">
@@ -765,12 +816,13 @@
         <v>0</v>
       </c>
       <c r="K6" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="3">
@@ -801,12 +853,13 @@
         <v>600</v>
       </c>
       <c r="K7" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="3">
@@ -837,53 +890,57 @@
         <v>600</v>
       </c>
       <c r="K8" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3600</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="3">
         <v>45026</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="5">
-        <v>6</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5">
-        <v>600</v>
-      </c>
-      <c r="K9" s="12">
-        <f t="shared" si="0"/>
-        <v>3600</v>
+      <c r="F9" s="2">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>45168</v>
+      </c>
+      <c r="J9" s="2">
+        <v>600</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="1"/>
+        <v>2400</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>45026</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>27</v>
@@ -907,89 +964,92 @@
         <v>600</v>
       </c>
       <c r="K10" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2400</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
+        <v>45178</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>45178</v>
+      </c>
+      <c r="J11" s="2">
+        <v>600</v>
+      </c>
+      <c r="K11" s="13">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
         <v>45026</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="5">
-        <v>4</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="F12" s="5">
+        <v>6</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H12" s="7">
         <v>0.3</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5">
-        <v>600</v>
-      </c>
-      <c r="K11" s="12">
-        <f t="shared" si="0"/>
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3">
-        <v>45026</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="2">
-        <v>4</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3">
-        <v>45168</v>
-      </c>
-      <c r="J12" s="2">
-        <v>600</v>
-      </c>
-      <c r="K12" s="13">
-        <f t="shared" si="0"/>
-        <v>2400</v>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5">
+        <v>600</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" ref="K12:K20" si="2">F12*J12</f>
+        <v>3600</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="6">
         <v>45026</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -998,7 +1058,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>23</v>
@@ -1011,31 +1071,815 @@
         <v>600</v>
       </c>
       <c r="K13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>45026</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="5">
+        <v>6</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5">
+        <v>600</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" si="2"/>
         <v>3600</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="14">
-        <f>SUM(K2:K13)</f>
-        <v>21000</v>
-      </c>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="14">
+        <v>45171</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="15">
+        <v>3</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15">
+        <v>600</v>
+      </c>
+      <c r="K15" s="16">
+        <f t="shared" si="2"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="14">
+        <v>45171</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="15">
+        <v>3</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15">
+        <v>600</v>
+      </c>
+      <c r="K16" s="16">
+        <f t="shared" si="2"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="14">
+        <v>45171</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="15">
+        <v>10</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15">
+        <v>600</v>
+      </c>
+      <c r="K17" s="16">
+        <f t="shared" si="2"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="14">
+        <v>45171</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="15">
+        <v>10</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15">
+        <v>600</v>
+      </c>
+      <c r="K18" s="16">
+        <f t="shared" si="2"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="14">
+        <v>45171</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="15">
+        <v>3</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15">
+        <v>600</v>
+      </c>
+      <c r="K19" s="16">
+        <f t="shared" si="2"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="14">
+        <v>45176</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="15">
+        <v>8</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15">
+        <v>600</v>
+      </c>
+      <c r="K20" s="16">
+        <f t="shared" si="2"/>
+        <v>4800</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6470C26-28B8-4261-BBE1-9EEABACD161C}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45026</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45168</v>
+      </c>
+      <c r="G2" s="2">
+        <v>600</v>
+      </c>
+      <c r="H2" s="18">
+        <f>D2*G2</f>
+        <v>3000</v>
+      </c>
+      <c r="I2" s="13">
+        <f>IF(E2="Completed",D2*G2,0)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:A17" si="0">+A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45026</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45168</v>
+      </c>
+      <c r="G3" s="2">
+        <v>600</v>
+      </c>
+      <c r="H3" s="18">
+        <f>D3*G3</f>
+        <v>2400</v>
+      </c>
+      <c r="I3" s="13">
+        <f>IF(E3="Completed",D3*G3,0)</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45026</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45168</v>
+      </c>
+      <c r="G4" s="2">
+        <v>600</v>
+      </c>
+      <c r="H4" s="18">
+        <f>D4*G4</f>
+        <v>2400</v>
+      </c>
+      <c r="I4" s="13">
+        <f>IF(E4="Completed",D4*G4,0)</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="14">
+        <v>45026</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="15">
+        <v>6</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15">
+        <v>600</v>
+      </c>
+      <c r="H5" s="19">
+        <f>D5*G5</f>
+        <v>3600</v>
+      </c>
+      <c r="I5" s="16">
+        <f>IF(E5="Completed",D5*G5,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="14">
+        <v>45026</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="15">
+        <v>4</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15">
+        <v>600</v>
+      </c>
+      <c r="H6" s="19">
+        <f>D6*G6</f>
+        <v>2400</v>
+      </c>
+      <c r="I6" s="16">
+        <f>IF(E6="Completed",D6*G6,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="14">
+        <v>45026</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="15">
+        <v>6</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15">
+        <v>600</v>
+      </c>
+      <c r="H7" s="19">
+        <f>D7*G7</f>
+        <v>3600</v>
+      </c>
+      <c r="I7" s="16">
+        <f>IF(E7="Completed",D7*G7,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45040</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3">
+        <v>45168</v>
+      </c>
+      <c r="G8" s="2">
+        <v>600</v>
+      </c>
+      <c r="H8" s="18">
+        <f>D8*G8</f>
+        <v>3600</v>
+      </c>
+      <c r="I8" s="13">
+        <f>IF(E8="Completed",D8*G8,0)</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45171</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3">
+        <v>45181</v>
+      </c>
+      <c r="G9" s="2">
+        <v>600</v>
+      </c>
+      <c r="H9" s="18">
+        <f>D9*G9</f>
+        <v>2400</v>
+      </c>
+      <c r="I9" s="13">
+        <f>IF(E9="Completed",D9*G9,0)</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>45171</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="15">
+        <v>10</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15">
+        <v>600</v>
+      </c>
+      <c r="H10" s="19">
+        <f>D10*G10</f>
+        <v>6000</v>
+      </c>
+      <c r="I10" s="16">
+        <f>IF(E10="Completed",D10*G10,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="14">
+        <v>45171</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15">
+        <v>600</v>
+      </c>
+      <c r="H11" s="19">
+        <f>D11*G11</f>
+        <v>6000</v>
+      </c>
+      <c r="I11" s="16">
+        <f>IF(E11="Completed",D11*G11,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="14">
+        <v>45171</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="15">
+        <v>3</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15">
+        <v>600</v>
+      </c>
+      <c r="H12" s="19">
+        <f>D12*G12</f>
+        <v>1800</v>
+      </c>
+      <c r="I12" s="16">
+        <f>IF(E12="Completed",D12*G12,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="14">
+        <v>45176</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="15">
+        <v>8</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15">
+        <v>600</v>
+      </c>
+      <c r="H13" s="19">
+        <f>D13*G13</f>
+        <v>4800</v>
+      </c>
+      <c r="I13" s="16">
+        <f>IF(E13="Completed",D13*G13,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="14">
+        <v>45176</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="15">
+        <v>8</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15">
+        <v>600</v>
+      </c>
+      <c r="H14" s="19">
+        <f>D14*G14</f>
+        <v>4800</v>
+      </c>
+      <c r="I14" s="16">
+        <f>IF(E14="Completed",D14*G14,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="14">
+        <v>45176</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="15">
+        <v>8</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15">
+        <v>600</v>
+      </c>
+      <c r="H15" s="19">
+        <f>D15*G15</f>
+        <v>4800</v>
+      </c>
+      <c r="I15" s="16">
+        <f>IF(E15="Completed",D15*G15,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45178</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="3">
+        <v>45178</v>
+      </c>
+      <c r="G16" s="2">
+        <v>600</v>
+      </c>
+      <c r="H16" s="18">
+        <f>D16*G16</f>
+        <v>600</v>
+      </c>
+      <c r="I16" s="13">
+        <f>IF(E16="Completed",D16*G16,0)</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="21">
+        <v>45178</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="20">
+        <v>2</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20">
+        <v>600</v>
+      </c>
+      <c r="H17" s="19">
+        <f>D17*G17</f>
+        <v>1200</v>
+      </c>
+      <c r="I17" s="16">
+        <f>IF(E17="Completed",D17*G17,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1">
+        <f>SUM(D2:D17)</f>
+        <v>89</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="17">
+        <f>SUM(H2:H17)</f>
+        <v>53400</v>
+      </c>
+      <c r="I18" s="17">
+        <f>SUM(I2:I17)</f>
+        <v>14400</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I17">
+    <sortCondition ref="B2:B17"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>